<commit_message>
Added Parallax to To-Do List
</commit_message>
<xml_diff>
--- a/Documents/To-Do List.xlsx
+++ b/Documents/To-Do List.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Desktop\Lusófona\2º Semestre\ProjectTallem\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{86C34DCF-E1D5-43AE-895E-D651138B467F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21576" windowHeight="8088" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="69">
   <si>
     <t>Conceitos</t>
   </si>
@@ -215,40 +224,47 @@
   </si>
   <si>
     <t>Conteudo Adicionado</t>
+  </si>
+  <si>
+    <t>Parallax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
-    <font/>
     <font>
-      <sz val="12.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF006100"/>
       <name val="Roboto"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF9C5700"/>
       <name val="Roboto"/>
     </font>
     <font>
       <b/>
+      <sz val="11"/>
       <color rgb="FF3C78D8"/>
       <name val="Roboto"/>
     </font>
@@ -258,7 +274,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -280,7 +296,13 @@
     </fill>
   </fills>
   <borders count="26">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF666666"/>
@@ -288,6 +310,9 @@
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -302,19 +327,23 @@
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF666666"/>
       </top>
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
@@ -324,6 +353,7 @@
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -332,14 +362,20 @@
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -351,10 +387,15 @@
       <top style="thin">
         <color rgb="FF666666"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -365,6 +406,7 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -374,14 +416,19 @@
         <color rgb="FF666666"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
+      <right/>
       <top style="thin">
         <color rgb="FF666666"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -393,11 +440,17 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -409,19 +462,28 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-    </border>
-    <border>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -430,19 +492,29 @@
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
-    </border>
-    <border>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color rgb="FF666666"/>
       </left>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -451,14 +523,20 @@
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -467,158 +545,461 @@
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
-    </border>
-    <border>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF666666"/>
       </right>
+      <top/>
       <bottom style="thin">
         <color rgb="FF666666"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="49">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="8" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="9" fillId="2" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="9" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="10" fillId="3" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="13" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="14" fillId="0" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="15" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="16" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="17" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="17" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="18" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="19" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="20" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="21" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="22" fillId="3" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="23" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
-    <xf borderId="24" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="25" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.57"/>
-    <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="33.86"/>
-    <col customWidth="1" min="4" max="4" width="42.0"/>
-    <col customWidth="1" min="5" max="5" width="30.71"/>
-    <col customWidth="1" min="6" max="8" width="8.71"/>
-    <col customWidth="1" min="9" max="9" width="19.57"/>
-    <col customWidth="1" min="10" max="27" width="8.71"/>
+    <col min="1" max="1" width="14.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" customWidth="1"/>
+    <col min="4" max="4" width="42" customWidth="1"/>
+    <col min="5" max="5" width="30.6640625" customWidth="1"/>
+    <col min="6" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="19.5546875" customWidth="1"/>
+    <col min="10" max="27" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.25" customHeight="1"/>
-    <row r="2" ht="14.25" customHeight="1">
+    <row r="1" spans="1:5" ht="14.25" customHeight="1"/>
+    <row r="2" spans="1:5" ht="14.25" customHeight="1">
       <c r="A2" s="1"/>
       <c r="B2" s="2" t="s">
         <v>0</v>
@@ -633,7 +1014,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" ht="14.25" customHeight="1">
+    <row r="3" spans="1:5" ht="14.25" customHeight="1">
       <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
@@ -641,336 +1022,340 @@
       <c r="D3" s="1"/>
       <c r="E3" s="8"/>
     </row>
-    <row r="4" ht="14.25" customHeight="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="8"/>
     </row>
-    <row r="5" ht="14.25" customHeight="1">
-      <c r="A5" s="1"/>
-      <c r="C5" s="13" t="s">
+    <row r="5" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A5" s="44"/>
+      <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>10</v>
       </c>
       <c r="E5" s="8"/>
     </row>
-    <row r="6" ht="14.25" customHeight="1">
-      <c r="A6" s="1"/>
-      <c r="C6" s="11" t="s">
+    <row r="6" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A6" s="44"/>
+      <c r="C6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>12</v>
       </c>
       <c r="E6" s="8"/>
     </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="14" t="s">
+    <row r="7" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A7" s="44"/>
+      <c r="B7" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="8"/>
     </row>
-    <row r="8" ht="14.25" customHeight="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="16" t="s">
+    <row r="8" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A8" s="44"/>
+      <c r="B8" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="17" t="s">
+      <c r="C8" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D8" s="17" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="8"/>
     </row>
-    <row r="9" ht="14.25" customHeight="1">
-      <c r="A9" s="1"/>
-      <c r="C9" s="17" t="s">
+    <row r="9" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A9" s="44"/>
+      <c r="C9" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="11" t="s">
         <v>20</v>
       </c>
       <c r="E9" s="8"/>
     </row>
-    <row r="10" ht="14.25" customHeight="1">
-      <c r="A10" s="1"/>
-      <c r="C10" s="17" t="s">
+    <row r="10" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A10" s="44"/>
+      <c r="C10" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="18" t="s">
+      <c r="D10" s="17" t="s">
         <v>22</v>
       </c>
       <c r="E10" s="8"/>
     </row>
-    <row r="11" ht="14.25" customHeight="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="14"/>
-      <c r="C11" s="13" t="s">
+    <row r="11" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A11" s="44"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="19" t="s">
+      <c r="D11" s="18" t="s">
         <v>24</v>
       </c>
       <c r="E11" s="8"/>
     </row>
-    <row r="12" ht="14.25" customHeight="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="14"/>
-      <c r="C12" s="13" t="s">
+    <row r="12" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A12" s="44"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="E12" s="8"/>
     </row>
-    <row r="13" ht="14.25" customHeight="1">
-      <c r="A13" s="20"/>
-      <c r="B13" s="14"/>
-      <c r="C13" s="17" t="s">
+    <row r="13" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A13" s="45"/>
+      <c r="B13" s="13"/>
+      <c r="C13" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>28</v>
       </c>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" ht="14.25" customHeight="1">
-      <c r="A14" s="22" t="s">
+    <row r="14" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A14" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="25" t="s">
+      <c r="D14" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="26"/>
-    </row>
-    <row r="15" ht="14.25" customHeight="1">
-      <c r="A15" s="27"/>
-      <c r="B15" s="28" t="s">
+      <c r="E14" s="23"/>
+    </row>
+    <row r="15" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A15" s="47"/>
+      <c r="B15" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="11" t="s">
         <v>35</v>
       </c>
       <c r="E15" s="8"/>
     </row>
-    <row r="16" ht="14.25" customHeight="1">
-      <c r="A16" s="27"/>
-      <c r="B16" s="29" t="s">
+    <row r="16" spans="1:5" ht="14.25" customHeight="1">
+      <c r="A16" s="47"/>
+      <c r="B16" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="17" t="s">
+      <c r="C16" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="30"/>
-    </row>
-    <row r="17" ht="14.25" customHeight="1">
-      <c r="A17" s="27"/>
-      <c r="B17" s="29" t="s">
+      <c r="E16" s="26"/>
+    </row>
+    <row r="17" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A17" s="47"/>
+      <c r="B17" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="17" t="s">
+      <c r="C17" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="11" t="s">
         <v>40</v>
       </c>
       <c r="E17" s="8"/>
     </row>
-    <row r="18" ht="14.25" customHeight="1">
-      <c r="A18" s="27"/>
-      <c r="B18" s="28"/>
-      <c r="C18" s="31" t="s">
+    <row r="18" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A18" s="47"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="32" t="s">
+      <c r="E18" s="28" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="19" ht="14.25" customHeight="1">
-      <c r="A19" s="27"/>
-      <c r="B19" s="28"/>
-      <c r="C19" s="17"/>
-      <c r="D19" s="18" t="s">
+    <row r="19" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A19" s="47"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="26" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" ht="14.25" customHeight="1">
-      <c r="A20" s="27"/>
-      <c r="B20" s="28"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="12" t="s">
+    <row r="20" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A20" s="47"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="26" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" ht="14.25" customHeight="1">
-      <c r="A21" s="33"/>
-      <c r="B21" s="34"/>
-      <c r="C21" s="35"/>
-      <c r="D21" s="36" t="s">
+    <row r="21" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A21" s="48"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="37" t="s">
+      <c r="E21" s="32" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" ht="14.25" customHeight="1">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A22" s="43" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="14"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="12" t="s">
+      <c r="B22" s="13"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="26" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="23" ht="14.25" customHeight="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="12" t="s">
+    <row r="23" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A23" s="44"/>
+      <c r="B23" s="13"/>
+      <c r="C23" s="16"/>
+      <c r="D23" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="32" t="s">
+      <c r="E23" s="28" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="24" ht="14.25" customHeight="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="14"/>
-      <c r="C24" s="17"/>
-      <c r="D24" s="12" t="s">
+    <row r="24" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A24" s="44"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="16"/>
+      <c r="D24" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E24" s="32" t="s">
+      <c r="E24" s="28" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" ht="14.25" customHeight="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="14"/>
-      <c r="C25" s="17"/>
-      <c r="D25" s="38" t="s">
+    <row r="25" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A25" s="44"/>
+      <c r="B25" s="13"/>
+      <c r="C25" s="16"/>
+      <c r="D25" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="E25" s="32" t="s">
+      <c r="E25" s="28" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="26" ht="14.25" customHeight="1">
-      <c r="A26" s="1"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="38" t="s">
+    <row r="26" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A26" s="44"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="16"/>
+      <c r="D26" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="E26" s="32" t="s">
+      <c r="E26" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="H26" s="39" t="s">
+      <c r="H26" s="34" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="27" ht="14.25" customHeight="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="38" t="s">
+    <row r="27" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A27" s="44"/>
+      <c r="B27" s="13"/>
+      <c r="C27" s="16"/>
+      <c r="D27" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="32" t="s">
+      <c r="E27" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="H27" s="40"/>
-      <c r="I27" s="39" t="s">
+      <c r="H27" s="35"/>
+      <c r="I27" s="34" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="28" ht="14.25" customHeight="1">
-      <c r="A28" s="1"/>
-      <c r="B28" s="14"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="32" t="s">
+    <row r="28" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A28" s="44"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E28" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="H28" s="41"/>
-      <c r="I28" s="39" t="s">
+      <c r="H28" s="36"/>
+      <c r="I28" s="34" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="29" ht="14.25" customHeight="1">
-      <c r="A29" s="1"/>
-      <c r="B29" s="14"/>
-      <c r="C29" s="17"/>
+    <row r="29" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A29" s="44"/>
+      <c r="B29" s="13"/>
+      <c r="C29" s="16"/>
       <c r="D29" s="7"/>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="28" t="s">
         <v>64</v>
       </c>
-      <c r="H29" s="42"/>
-      <c r="I29" s="39" t="s">
+      <c r="H29" s="37"/>
+      <c r="I29" s="34" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="30" ht="14.25" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="46"/>
-      <c r="H30" s="47" t="s">
+    <row r="30" spans="1:9" ht="14.25" customHeight="1">
+      <c r="A30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="39"/>
+      <c r="D30" s="40"/>
+      <c r="E30" s="41"/>
+      <c r="H30" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="I30" s="39" t="s">
+      <c r="I30" s="34" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="31" spans="1:9" ht="14.25" customHeight="1"/>
+    <row r="32" spans="1:9" ht="14.25" customHeight="1"/>
     <row r="33" ht="14.25" customHeight="1"/>
     <row r="34" ht="14.25" customHeight="1"/>
     <row r="35" ht="14.25" customHeight="1"/>
@@ -1945,9 +2330,7 @@
     <mergeCell ref="A14:A21"/>
     <mergeCell ref="A22:A30"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>